<commit_message>
Updated dates in Brian Bunting Collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/BRIAN BUNTING COLLECTION.xlsx
+++ b/Photographic Archive/BRIAN BUNTING COLLECTION.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1222,6 +1225,7 @@
       <c r="G68" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed acquisition date from Brian Bunting Collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/BRIAN BUNTING COLLECTION.xlsx
+++ b/Photographic Archive/BRIAN BUNTING COLLECTION.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>identifier</t>
   </si>
@@ -43,24 +43,9 @@
     <t>file_path</t>
   </si>
   <si>
-    <t>ACCESSION NO</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>ACQUISITION NO.</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
-    <t>ITEM DESCRIPTION</t>
-  </si>
-  <si>
-    <t>LOCATION | SECTION</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -77,9 +62,6 @@
   </si>
   <si>
     <t>Funeral and Memorial Services/Moses Kotane PHOTOGRAPH</t>
-  </si>
-  <si>
-    <t>01/04/2014</t>
   </si>
   <si>
     <t>PHOTOGRAPH</t>
@@ -125,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,21 +130,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -212,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -222,30 +189,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -467,11 +421,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z68"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -481,9 +435,10 @@
     <col min="3" max="3" width="47" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" customWidth="1"/>
-    <col min="8" max="9" width="92.33203125" customWidth="1"/>
-    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="11" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -513,10 +468,18 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -531,210 +494,172 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>8</v>
+      <c r="A2" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8">
+        <v>1</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="N2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="12"/>
+      <c r="N3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8">
+        <v>1</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12">
+      <c r="M4" s="12"/>
+      <c r="N4" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8">
         <v>1</v>
       </c>
-      <c r="L3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="M5" s="12"/>
+      <c r="N5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8">
         <v>1</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12">
-        <v>1</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="16"/>
-      <c r="N5" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12">
-        <v>1</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12">
-        <v>1</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="M6" s="12"/>
+      <c r="N6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -888,7 +813,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
@@ -1216,14 +1141,6 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:Z1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>